<commit_message>
Added file to create tables. Updated excel to be in line with our model. Fixed inserts
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\IdeaProjects\sem3pi2024_25_g125\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B12CC5-064E-4E27-AAF7-867BB8C140FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4407BEF-298D-42D2-ACDB-84D12D351A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="8" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="205">
   <si>
     <t>Name</t>
   </si>
@@ -577,9 +577,6 @@
     <t>ProductFamily</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>Delivery</t>
   </si>
   <si>
@@ -616,12 +613,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Order_ID</t>
-  </si>
-  <si>
     <t>customer_nif</t>
   </si>
   <si>
@@ -656,6 +647,18 @@
   </si>
   <si>
     <t>SQL</t>
+  </si>
+  <si>
+    <t>Location_address</t>
+  </si>
+  <si>
+    <t>Location_zip</t>
+  </si>
+  <si>
+    <t>ClientOrder</t>
+  </si>
+  <si>
+    <t>OrderID</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D52B8C6-F495-435D-B053-FB604FC6DD2C}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="D1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1051,10 +1054,12 @@
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="87.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="130.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>166</v>
       </c>
@@ -1089,16 +1094,22 @@
         <v>174</v>
       </c>
       <c r="L1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M1" t="s">
         <v>185</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>186</v>
       </c>
-      <c r="N1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>456</v>
       </c>
@@ -1127,15 +1138,15 @@
         <v>153</v>
       </c>
       <c r="J2" t="str">
-        <f>"INSERT INTO " &amp; $J$1 &amp; "(" &amp; $M$1 &amp; ", " &amp;$E$1 &amp; ", " &amp;$F$1 &amp; ", " &amp;$G$1 &amp; ") values ('" &amp; E2 &amp; "', '" &amp; F2 &amp; "', '" &amp; G2 &amp; "');"</f>
-        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('4200-047', 'Porto', 'Portugal');</v>
+        <f>"INSERT INTO " &amp; $J$1 &amp; "(" &amp; $M$1 &amp; ", " &amp;$E$1 &amp; ", " &amp;$F$1 &amp; ", " &amp;$G$1 &amp; ") values ('" &amp; D2 &amp; "', '" &amp; E2 &amp; "', '" &amp; F2 &amp; "', '" &amp; G2 &amp; "');"</f>
+        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('Tv. Augusto Lessa 23', '4200-047', 'Porto', 'Portugal');</v>
       </c>
       <c r="K2" t="str">
-        <f>"INSERT INTO " &amp; $K$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$M$1 &amp; ", " &amp;$H$1 &amp; ", " &amp;$N$1 &amp; ") values (" &amp;A2 &amp; ", '" &amp; B2 &amp; "', '" &amp; C2 &amp; "', '" &amp; D2 &amp; "', '" &amp; H2 &amp; "', " &amp; I2 &amp; ");"</f>
-        <v>INSERT INTO Customer(nif, Name, VATIN, address, Email, phoneNumber) values (456, 'Carvalho &amp; Carvalho, Lda', 'PT501245987', 'Tv. Augusto Lessa 23', 'idont@care.com', 003518340500);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $K$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$O$1 &amp; ", " &amp;$P$1 &amp; ", " &amp;$H$1 &amp; ", " &amp;$N$1 &amp; ") values (" &amp;A2 &amp; ", '" &amp; B2 &amp; "', '" &amp; C2 &amp; "', '" &amp; D2 &amp; "', '" &amp; E2 &amp; "', '" &amp; H2 &amp; "', " &amp; I2 &amp; ");"</f>
+        <v>INSERT INTO Customer(nif, Name, VATIN, Location_address, Location_zip, Email, phoneNumber) values (456, 'Carvalho &amp; Carvalho, Lda', 'PT501245987', 'Tv. Augusto Lessa 23', '4200-047', 'idont@care.com', 003518340500);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>785</v>
       </c>
@@ -1164,15 +1175,15 @@
         <v>153</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J5" si="0">"INSERT INTO " &amp; $J$1 &amp; "(" &amp; $M$1 &amp; ", " &amp;$E$1 &amp; ", " &amp;$F$1 &amp; ", " &amp;$G$1 &amp; ") values ('" &amp; E3 &amp; "', '" &amp; F3 &amp; "', '" &amp; G3 &amp; "');"</f>
-        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('4465-219', 'São Mamede de Infesta', 'Portugal');</v>
+        <f t="shared" ref="J3:J5" si="0">"INSERT INTO " &amp; $J$1 &amp; "(" &amp; $M$1 &amp; ", " &amp;$E$1 &amp; ", " &amp;$F$1 &amp; ", " &amp;$G$1 &amp; ") values ('" &amp; D3 &amp; "', '" &amp; E3 &amp; "', '" &amp; F3 &amp; "', '" &amp; G3 &amp; "');"</f>
+        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('R. Dr. Barros 93', '4465-219', 'São Mamede de Infesta', 'Portugal');</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K5" si="1">"INSERT INTO " &amp; $K$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$M$1 &amp; ", " &amp;$H$1 &amp; ", " &amp;$N$1 &amp; ") values (" &amp;A3 &amp; ", '" &amp; B3 &amp; "', '" &amp; C3 &amp; "', '" &amp; D3 &amp; "', '" &amp; H3 &amp; "', " &amp; I3 &amp; ");"</f>
-        <v>INSERT INTO Customer(nif, Name, VATIN, address, Email, phoneNumber) values (785, 'Tudo para a casa, Lda', 'PT501245488', 'R. Dr. Barros 93', 'me@neither.com', 003518340500);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K3:K5" si="1">"INSERT INTO " &amp; $K$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$O$1 &amp; ", " &amp;$P$1 &amp; ", " &amp;$H$1 &amp; ", " &amp;$N$1 &amp; ") values (" &amp;A3 &amp; ", '" &amp; B3 &amp; "', '" &amp; C3 &amp; "', '" &amp; D3 &amp; "', '" &amp; E3 &amp; "', '" &amp; H3 &amp; "', " &amp; I3 &amp; ");"</f>
+        <v>INSERT INTO Customer(nif, Name, VATIN, Location_address, Location_zip, Email, phoneNumber) values (785, 'Tudo para a casa, Lda', 'PT501245488', 'R. Dr. Barros 93', '4465-219', 'me@neither.com', 003518340500);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>657</v>
       </c>
@@ -1202,14 +1213,14 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('4400-023', 'Vila Nova de Gaia', 'Portugal');</v>
+        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('EDIFICIO CRISTAL lj18, R. António Correia de Carvalho 88', '4400-023', 'Vila Nova de Gaia', 'Portugal');</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Customer(nif, Name, VATIN, address, Email, phoneNumber) values (657, 'Sair de Cena', 'PT501242417', 'EDIFICIO CRISTAL lj18, R. António Correia de Carvalho 88', 'some@email.com', 003518340500);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>INSERT INTO Customer(nif, Name, VATIN, Location_address, Location_zip, Email, phoneNumber) values (657, 'Sair de Cena', 'PT501242417', 'EDIFICIO CRISTAL lj18, R. António Correia de Carvalho 88', '4400-023', 'some@email.com', 003518340500);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>348</v>
       </c>
@@ -1239,11 +1250,11 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('110 00', 'Nové Město', 'Czechia');</v>
+        <v>INSERT INTO Location(address, ZIP, Town, Country) values ('Křemencova 11', '110 00', 'Nové Město', 'Czechia');</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Customer(nif, Name, VATIN, address, Email, phoneNumber) values (348, 'U Fleku', 'CZ6451237810', 'Křemencova 11', 'some.random@email.cz', 004201234567);</v>
+        <v>INSERT INTO Customer(nif, Name, VATIN, Location_address, Location_zip, Email, phoneNumber) values (348, 'U Fleku', 'CZ6451237810', 'Křemencova 11', '110 00', 'some.random@email.cz', 004201234567);</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1268,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,10 +1292,10 @@
         <v>145</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H1" t="s">
         <v>127</v>
@@ -1304,7 +1315,7 @@
         <v>130</v>
       </c>
       <c r="E2" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A2 &amp; "', '" &amp; B2 &amp; "', '" &amp; C2 &amp; "', " &amp; D2 &amp; ");"</f>
+        <f t="shared" ref="E2:E8" si="0">"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A2 &amp; "', '" &amp; B2 &amp; "', '" &amp; C2 &amp; "', " &amp; D2 &amp; ");"</f>
         <v>INSERT INTO Product(Code, Name, Description, productFamily_ID) values ('AS12945T22', 'La Belle 22 5l pot', '5l 22 cm aluminium and teflon non stick pot', 130);</v>
       </c>
     </row>
@@ -1322,7 +1333,7 @@
         <v>125</v>
       </c>
       <c r="E3" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A3 &amp; "', '" &amp; B3 &amp; "', '" &amp; C3 &amp; "', " &amp; D3 &amp; ");"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product(Code, Name, Description, productFamily_ID) values ('AS12945S22', 'Pro 22 5l pot', '5l 22 cm stainless steel pot', 125);</v>
       </c>
     </row>
@@ -1340,7 +1351,7 @@
         <v>125</v>
       </c>
       <c r="E4" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A4 &amp; "', '" &amp; B4 &amp; "', '" &amp; C4 &amp; "', " &amp; D4 &amp; ");"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product(Code, Name, Description, productFamily_ID) values ('AS12945S20', 'Pro 20 3l pot', '3l 20 cm stainless steel pot', 125);</v>
       </c>
     </row>
@@ -1358,7 +1369,7 @@
         <v>125</v>
       </c>
       <c r="E5" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A5 &amp; "', '" &amp; B5 &amp; "', '" &amp; C5 &amp; "', " &amp; D5 &amp; ");"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product(Code, Name, Description, productFamily_ID) values ('AS12945S17', 'Pro 17 2l pot', '2l 17 cm stainless steel pot', 125);</v>
       </c>
     </row>
@@ -1376,7 +1387,7 @@
         <v>132</v>
       </c>
       <c r="E6" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A6 &amp; "', '" &amp; B6 &amp; "', '" &amp; C6 &amp; "', " &amp; D6 &amp; ");"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product(Code, Name, Description, productFamily_ID) values ('AS12945P17', 'Pro 17 2l sauce pan', '2l 17 cm stainless steel souce pan', 132);</v>
       </c>
     </row>
@@ -1394,7 +1405,7 @@
         <v>145</v>
       </c>
       <c r="E7" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A7 &amp; "', '" &amp; B7 &amp; "', '" &amp; C7 &amp; "', " &amp; D7 &amp; ");"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product(Code, Name, Description, productFamily_ID) values ('AS12945S48', 'Pro 17 lid', '17 cm stainless steel lid', 145);</v>
       </c>
     </row>
@@ -1412,7 +1423,7 @@
         <v>146</v>
       </c>
       <c r="E8" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $A$1 &amp; ", " &amp;$B$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$F$1 &amp; ") values ('" &amp;A8 &amp; "', '" &amp; B8 &amp; "', '" &amp; C8 &amp; "', " &amp; D8 &amp; ");"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product(Code, Name, Description, productFamily_ID) values ('AS12945G48', 'Pro Clear 17 lid', '17 cm glass lid', 146);</v>
       </c>
     </row>
@@ -1426,7 +1437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A03423-14BC-4B6A-8318-AD0C48152F2D}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1446,7 +1457,7 @@
         <v>176</v>
       </c>
       <c r="E1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1516,10 +1527,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE470C24-4865-4CED-BECB-9AD0BD718C1F}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,13 +1538,13 @@
     <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="69.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="89.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="94.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -1553,31 +1564,28 @@
         <v>129</v>
       </c>
       <c r="G1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" t="s">
         <v>177</v>
       </c>
-      <c r="H1" t="s">
-        <v>178</v>
-      </c>
       <c r="I1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L1" t="s">
         <v>189</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>190</v>
       </c>
-      <c r="L1" t="s">
-        <v>191</v>
-      </c>
-      <c r="M1" t="s">
-        <v>192</v>
-      </c>
-      <c r="N1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1597,19 +1605,19 @@
         <v>45558</v>
       </c>
       <c r="G2" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $K$1 &amp;") values (" &amp;A2 &amp; ", " &amp; B2 &amp; ", '" &amp; TEXT(E2, "DD/MM/AAAA") &amp; "');"</f>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (1, 785, '15/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A2 &amp; ", " &amp; B2 &amp; ", TO_DATE('" &amp; TEXT(E2, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (1, 785, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H2" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $K$1 &amp; ") values (" &amp;A2 &amp; ", '" &amp; C2 &amp; "', '" &amp; TEXT(F2, "DD/MM/AAAA") &amp; "');"</f>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (1, 'AS12945S22', '23/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A2 &amp; ", " &amp; B2 &amp; ", TO_DATE('" &amp; TEXT(F2, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (1, 785, TO_DATE('23/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I2" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$N$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A2 &amp; ", '" &amp; C2 &amp; "', " &amp; D2 &amp; ");"</f>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (1, 'AS12945S22', 5);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A2 &amp; ", '" &amp; C2 &amp; "', " &amp; D2 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (1, 'AS12945S22', 5);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1629,19 +1637,19 @@
         <v>45558</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G14" si="0">"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $K$1 &amp;") values (" &amp;A3 &amp; ", " &amp; B3 &amp; ", '" &amp; TEXT(E3, "DD/MM/AAAA") &amp; "');"</f>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (1, 785, '15/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A3 &amp; ", " &amp; B3 &amp; ", TO_DATE('" &amp; TEXT(E3, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (1, 785, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H14" si="1">"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $K$1 &amp; ") values (" &amp;A3 &amp; ", '" &amp; C3 &amp; "', '" &amp; TEXT(F3, "DD/MM/AAAA") &amp; "');"</f>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (1, 'AS12945S20', '23/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A3 &amp; ", " &amp; B3 &amp; ", TO_DATE('" &amp; TEXT(F3, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (1, 785, TO_DATE('23/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I14" si="2">"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$N$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A3 &amp; ", '" &amp; C3 &amp; "', " &amp; D3 &amp; ");"</f>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (1, 'AS12945S20', 15);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A3 &amp; ", '" &amp; C3 &amp; "', " &amp; D3 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (1, 'AS12945S20', 15);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1661,19 +1669,19 @@
         <v>45561</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (2, 657, '15/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A4 &amp; ", " &amp; B4 &amp; ", TO_DATE('" &amp; TEXT(E4, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (2, 657, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (2, 'AS12945S22', '26/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A4 &amp; ", " &amp; B4 &amp; ", TO_DATE('" &amp; TEXT(F4, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (2, 657, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (2, 'AS12945S22', 10);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A4 &amp; ", '" &amp; C4 &amp; "', " &amp; D4 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (2, 'AS12945S22', 10);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1693,19 +1701,19 @@
         <v>45561</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (2, 657, '15/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A5 &amp; ", " &amp; B5 &amp; ", TO_DATE('" &amp; TEXT(E5, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (2, 657, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (2, 'AS12945P17', '26/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A5 &amp; ", " &amp; B5 &amp; ", TO_DATE('" &amp; TEXT(F5, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (2, 657, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (2, 'AS12945P17', 20);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A5 &amp; ", '" &amp; C5 &amp; "', " &amp; D5 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (2, 'AS12945P17', 20);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1725,19 +1733,19 @@
         <v>45560</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (3, 348, '15/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A6 &amp; ", " &amp; B6 &amp; ", TO_DATE('" &amp; TEXT(E6, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (3, 348, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (3, 'AS12945S22', '25/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A6 &amp; ", " &amp; B6 &amp; ", TO_DATE('" &amp; TEXT(F6, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (3, 348, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (3, 'AS12945S22', 10);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A6 &amp; ", '" &amp; C6 &amp; "', " &amp; D6 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (3, 'AS12945S22', 10);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1757,19 +1765,19 @@
         <v>45560</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (3, 348, '15/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A7 &amp; ", " &amp; B7 &amp; ", TO_DATE('" &amp; TEXT(E7, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (3, 348, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (3, 'AS12945S20', '25/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A7 &amp; ", " &amp; B7 &amp; ", TO_DATE('" &amp; TEXT(F7, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (3, 348, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (3, 'AS12945S20', 10);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A7 &amp; ", '" &amp; C7 &amp; "', " &amp; D7 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (3, 'AS12945S20', 10);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1789,19 +1797,19 @@
         <v>45560</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (4, 785, '18/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A8 &amp; ", " &amp; B8 &amp; ", TO_DATE('" &amp; TEXT(E8, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (4, 785, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (4, 'AS12945S20', '25/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A8 &amp; ", " &amp; B8 &amp; ", TO_DATE('" &amp; TEXT(F8, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (4, 785, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (4, 'AS12945S20', 24);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A8 &amp; ", '" &amp; C8 &amp; "', " &amp; D8 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (4, 'AS12945S20', 24);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1821,19 +1829,19 @@
         <v>45560</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (4, 785, '18/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A9 &amp; ", " &amp; B9 &amp; ", TO_DATE('" &amp; TEXT(E9, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (4, 785, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (4, 'AS12945S22', '25/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A9 &amp; ", " &amp; B9 &amp; ", TO_DATE('" &amp; TEXT(F9, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (4, 785, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (4, 'AS12945S22', 16);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A9 &amp; ", '" &amp; C9 &amp; "', " &amp; D9 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (4, 'AS12945S22', 16);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1853,19 +1861,19 @@
         <v>45560</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (4, 785, '18/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A10 &amp; ", " &amp; B10 &amp; ", TO_DATE('" &amp; TEXT(E10, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (4, 785, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (4, 'AS12945S17', '25/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A10 &amp; ", " &amp; B10 &amp; ", TO_DATE('" &amp; TEXT(F10, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (4, 785, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (4, 'AS12945S17', 8);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A10 &amp; ", '" &amp; C10 &amp; "', " &amp; D10 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (4, 'AS12945S17', 8);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1885,19 +1893,19 @@
         <v>45560</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (5, 657, '18/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A11 &amp; ", " &amp; B11 &amp; ", TO_DATE('" &amp; TEXT(E11, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (5, 657, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (5, 'AS12945S22', '25/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A11 &amp; ", " &amp; B11 &amp; ", TO_DATE('" &amp; TEXT(F11, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (5, 657, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (5, 'AS12945S22', 12);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A11 &amp; ", '" &amp; C11 &amp; "', " &amp; D11 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (5, 'AS12945S22', 12);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1917,19 +1925,19 @@
         <v>45561</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (6, 348, '18/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A12 &amp; ", " &amp; B12 &amp; ", TO_DATE('" &amp; TEXT(E12, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (6, 348, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (6, 'AS12945S17', '26/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A12 &amp; ", " &amp; B12 &amp; ", TO_DATE('" &amp; TEXT(F12, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (6, 348, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (6, 'AS12945S17', 8);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A12 &amp; ", '" &amp; C12 &amp; "', " &amp; D12 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (6, 'AS12945S17', 8);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1949,19 +1957,19 @@
         <v>45561</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (6, 348, '18/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A13 &amp; ", " &amp; B13 &amp; ", TO_DATE('" &amp; TEXT(E13, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (6, 348, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (6, 'AS12945P17', '26/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A13 &amp; ", " &amp; B13 &amp; ", TO_DATE('" &amp; TEXT(F13, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (6, 348, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (6, 'AS12945P17', 16);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A13 &amp; ", '" &amp; C13 &amp; "', " &amp; D13 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (6, 'AS12945P17', 16);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1981,16 +1989,16 @@
         <v>45561</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Order(ID, customer_nif, date) values (7, 456, '21/09/2024');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A14 &amp; ", " &amp; B14 &amp; ", TO_DATE('" &amp; TEXT(E14, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (7, 456, TO_DATE('21/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Delivery(Order_ID, customer_nif, date) values (7, 'AS12945S22', '26/09/2024');</v>
+        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A14 &amp; ", " &amp; B14 &amp; ", TO_DATE('" &amp; TEXT(F14, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (7, 456, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(ID, productcode, Quantity) values (7, 'AS12945S22', 8);</v>
+        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A14 &amp; ", '" &amp; C14 &amp; "', " &amp; D14 &amp; ");"</f>
+        <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (7, 'AS12945S22', 8);</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2011,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,22 +2041,22 @@
         <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="M1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2072,10 +2080,10 @@
         <v>INSERT INTO Operation(ID, Description) values (5647, 'Disc cutting');</v>
       </c>
       <c r="G2" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$J$1 &amp; ") values (" &amp; A2 &amp; ", '" &amp; C2 &amp; "')" &amp;
-IF(D2&lt;&gt;"", ", (" &amp; A2 &amp; ",'" &amp; D2 &amp; "')", "") &amp;
-IF(E2&lt;&gt;"", ", (" &amp; A2 &amp; ", '" &amp; E2 &amp; "')", "") &amp; ";"</f>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5647, 'A4578'), (5647,'A4588'), (5647, 'A4598');</v>
+        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp; $J$1 &amp; ") VALUES (" &amp; A2 &amp; ", '" &amp; C2 &amp; "');" &amp;
+IF(D2&lt;&gt;"", " INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp; $J$1 &amp; ") VALUES (" &amp; A2 &amp; ", '" &amp; D2 &amp; "');", "") &amp;
+IF(E2&lt;&gt;"", " INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp; $J$1 &amp; ") VALUES (" &amp; A2 &amp; ", '" &amp; E2 &amp; "');", "")</f>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5647, 'A4578'); INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5647, 'A4588'); INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5647, 'A4598');</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -2096,10 +2104,10 @@
         <v>INSERT INTO Operation(ID, Description) values (5649, 'Initial pot base pressing');</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G19" si="1">"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp;$J$1 &amp; ") values (" &amp; A3 &amp; ", '" &amp; C3 &amp; "')" &amp;
-IF(D3&lt;&gt;"", ", (" &amp; A3 &amp; ",'" &amp; D3 &amp; "')", "") &amp;
-IF(E3&lt;&gt;"", ", (" &amp; A3 &amp; ", '" &amp; E3 &amp; "')", "") &amp; ";"</f>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5649, 'A4588'), (5649,'A4598');</v>
+        <f t="shared" ref="G3:G19" si="1">"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp; $J$1 &amp; ") VALUES (" &amp; A3 &amp; ", '" &amp; C3 &amp; "');" &amp;
+IF(D3&lt;&gt;"", " INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp; $J$1 &amp; ") VALUES (" &amp; A3 &amp; ", '" &amp; D3 &amp; "');", "") &amp;
+IF(E3&lt;&gt;"", " INSERT INTO " &amp; $G$1 &amp; "(" &amp; $L$1 &amp; ", " &amp; $J$1 &amp; ") VALUES (" &amp; A3 &amp; ", '" &amp; E3 &amp; "');", "")</f>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5649, 'A4588'); INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5649, 'A4598');</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -2121,7 +2129,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5651, 'A4588'), (5651,'A4598');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5651, 'A4588'); INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5651, 'A4598');</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2140,7 +2148,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5653, 'C5637');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5653, 'C5637');</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -2162,7 +2170,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5655, 'A4588'), (5655,'A4598');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5655, 'A4588'); INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5655, 'A4598');</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -2181,7 +2189,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5657, 'C5637');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5657, 'C5637');</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -2200,7 +2208,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5659, 'S3271');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5659, 'S3271');</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -2219,7 +2227,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5661, 'T3452');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5661, 'T3452');</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -2238,7 +2246,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5663, 'K3675');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5663, 'K3675');</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -2257,7 +2265,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5665, 'D9123');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5665, 'D9123');</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -2276,7 +2284,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5667, 'Q3547');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5667, 'Q3547');</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2295,7 +2303,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5669, 'Q3547');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5669, 'Q3547');</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -2314,7 +2322,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5671, 'Q5478');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5671, 'Q5478');</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -2336,7 +2344,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5681, 'A4588'), (5681,'A4598');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5681, 'A4588'); INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5681, 'A4598');</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2358,7 +2366,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5682, 'A4588'), (5682,'A4598');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5682, 'A4588'); INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5682, 'A4598');</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2377,7 +2385,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5683, 'C5637');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5683, 'C5637');</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2396,7 +2404,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5665, 'D9123');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5665, 'D9123');</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2415,7 +2423,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) values (5688, 'K3675');</v>
+        <v>INSERT INTO Operation_WorkstationType(Operation_ID, WorkstationType_ID) VALUES (5688, 'K3675');</v>
       </c>
     </row>
   </sheetData>
@@ -2446,13 +2454,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D1" t="s">
         <v>141</v>
       </c>
       <c r="E1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2645,13 +2653,13 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3069,19 +3077,19 @@
         <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -3533,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B436D-7E6F-45CD-A274-6E2AE1A9129E}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3557,16 +3565,16 @@
         <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed an issue with the Delivery table values being inserted
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\IdeaProjects\sem3pi2024_25_g125\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4407BEF-298D-42D2-ACDB-84D12D351A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD4496-CE93-499E-AEB3-085C8EF13DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="8" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -1529,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE470C24-4865-4CED-BECB-9AD0BD718C1F}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1605,15 +1605,15 @@
         <v>45558</v>
       </c>
       <c r="G2" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A2 &amp; ", " &amp; B2 &amp; ", TO_DATE('" &amp; TEXT(E2, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" ref="G2:G14" si="0">"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A2 &amp; ", " &amp; B2 &amp; ", TO_DATE('" &amp; TEXT(E2, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (1, 785, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H2" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A2 &amp; ", " &amp; B2 &amp; ", TO_DATE('" &amp; TEXT(F2, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" ref="H2:H14" si="1">"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A2 &amp; ", " &amp; B2 &amp; ", TO_DATE('" &amp; TEXT(F2, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (1, 785, TO_DATE('23/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I2" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A2 &amp; ", '" &amp; C2 &amp; "', " &amp; D2 &amp; ");"</f>
+        <f t="shared" ref="I2:I14" si="2">"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A2 &amp; ", '" &amp; C2 &amp; "', " &amp; D2 &amp; ");"</f>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (1, 'AS12945S22', 5);</v>
       </c>
     </row>
@@ -1637,15 +1637,15 @@
         <v>45558</v>
       </c>
       <c r="G3" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A3 &amp; ", " &amp; B3 &amp; ", TO_DATE('" &amp; TEXT(E3, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (1, 785, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H3" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A3 &amp; ", " &amp; B3 &amp; ", TO_DATE('" &amp; TEXT(F3, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (1, 785, TO_DATE('23/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I3" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A3 &amp; ", '" &amp; C3 &amp; "', " &amp; D3 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (1, 'AS12945S20', 15);</v>
       </c>
     </row>
@@ -1669,15 +1669,15 @@
         <v>45561</v>
       </c>
       <c r="G4" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A4 &amp; ", " &amp; B4 &amp; ", TO_DATE('" &amp; TEXT(E4, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (2, 657, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H4" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A4 &amp; ", " &amp; B4 &amp; ", TO_DATE('" &amp; TEXT(F4, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (2, 657, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I4" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A4 &amp; ", '" &amp; C4 &amp; "', " &amp; D4 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (2, 'AS12945S22', 10);</v>
       </c>
     </row>
@@ -1701,15 +1701,15 @@
         <v>45561</v>
       </c>
       <c r="G5" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A5 &amp; ", " &amp; B5 &amp; ", TO_DATE('" &amp; TEXT(E5, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (2, 657, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H5" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A5 &amp; ", " &amp; B5 &amp; ", TO_DATE('" &amp; TEXT(F5, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (2, 657, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I5" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A5 &amp; ", '" &amp; C5 &amp; "', " &amp; D5 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (2, 'AS12945P17', 20);</v>
       </c>
     </row>
@@ -1733,15 +1733,15 @@
         <v>45560</v>
       </c>
       <c r="G6" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A6 &amp; ", " &amp; B6 &amp; ", TO_DATE('" &amp; TEXT(E6, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (3, 348, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H6" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A6 &amp; ", " &amp; B6 &amp; ", TO_DATE('" &amp; TEXT(F6, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (3, 348, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I6" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A6 &amp; ", '" &amp; C6 &amp; "', " &amp; D6 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (3, 'AS12945S22', 10);</v>
       </c>
     </row>
@@ -1765,15 +1765,15 @@
         <v>45560</v>
       </c>
       <c r="G7" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A7 &amp; ", " &amp; B7 &amp; ", TO_DATE('" &amp; TEXT(E7, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (3, 348, TO_DATE('15/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H7" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A7 &amp; ", " &amp; B7 &amp; ", TO_DATE('" &amp; TEXT(F7, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (3, 348, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I7" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A7 &amp; ", '" &amp; C7 &amp; "', " &amp; D7 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (3, 'AS12945S20', 10);</v>
       </c>
     </row>
@@ -1797,15 +1797,15 @@
         <v>45560</v>
       </c>
       <c r="G8" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A8 &amp; ", " &amp; B8 &amp; ", TO_DATE('" &amp; TEXT(E8, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (4, 785, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H8" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A8 &amp; ", " &amp; B8 &amp; ", TO_DATE('" &amp; TEXT(F8, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (4, 785, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I8" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A8 &amp; ", '" &amp; C8 &amp; "', " &amp; D8 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (4, 'AS12945S20', 24);</v>
       </c>
     </row>
@@ -1829,15 +1829,15 @@
         <v>45560</v>
       </c>
       <c r="G9" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A9 &amp; ", " &amp; B9 &amp; ", TO_DATE('" &amp; TEXT(E9, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (4, 785, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H9" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A9 &amp; ", " &amp; B9 &amp; ", TO_DATE('" &amp; TEXT(F9, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (4, 785, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I9" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A9 &amp; ", '" &amp; C9 &amp; "', " &amp; D9 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (4, 'AS12945S22', 16);</v>
       </c>
     </row>
@@ -1861,15 +1861,15 @@
         <v>45560</v>
       </c>
       <c r="G10" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A10 &amp; ", " &amp; B10 &amp; ", TO_DATE('" &amp; TEXT(E10, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (4, 785, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H10" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A10 &amp; ", " &amp; B10 &amp; ", TO_DATE('" &amp; TEXT(F10, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (4, 785, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I10" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A10 &amp; ", '" &amp; C10 &amp; "', " &amp; D10 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (4, 'AS12945S17', 8);</v>
       </c>
     </row>
@@ -1893,15 +1893,15 @@
         <v>45560</v>
       </c>
       <c r="G11" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A11 &amp; ", " &amp; B11 &amp; ", TO_DATE('" &amp; TEXT(E11, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (5, 657, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H11" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A11 &amp; ", " &amp; B11 &amp; ", TO_DATE('" &amp; TEXT(F11, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (5, 657, TO_DATE('25/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I11" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A11 &amp; ", '" &amp; C11 &amp; "', " &amp; D11 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (5, 'AS12945S22', 12);</v>
       </c>
     </row>
@@ -1925,15 +1925,15 @@
         <v>45561</v>
       </c>
       <c r="G12" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A12 &amp; ", " &amp; B12 &amp; ", TO_DATE('" &amp; TEXT(E12, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (6, 348, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H12" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A12 &amp; ", " &amp; B12 &amp; ", TO_DATE('" &amp; TEXT(F12, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (6, 348, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I12" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A12 &amp; ", '" &amp; C12 &amp; "', " &amp; D12 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (6, 'AS12945S17', 8);</v>
       </c>
     </row>
@@ -1957,15 +1957,15 @@
         <v>45561</v>
       </c>
       <c r="G13" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A13 &amp; ", " &amp; B13 &amp; ", TO_DATE('" &amp; TEXT(E13, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (6, 348, TO_DATE('18/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H13" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A13 &amp; ", " &amp; B13 &amp; ", TO_DATE('" &amp; TEXT(F13, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (6, 348, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I13" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A13 &amp; ", '" &amp; C13 &amp; "', " &amp; D13 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (6, 'AS12945P17', 16);</v>
       </c>
     </row>
@@ -1989,15 +1989,15 @@
         <v>45561</v>
       </c>
       <c r="G14" t="str">
-        <f>"INSERT INTO " &amp; $G$1 &amp; "(" &amp; $J$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $E$1 &amp;") values (" &amp;A14 &amp; ", " &amp; B14 &amp; ", TO_DATE('" &amp; TEXT(E14, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ClientOrder(ID, customer_nif, DateOrder) values (7, 456, TO_DATE('21/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="H14" t="str">
-        <f>"INSERT INTO " &amp; $H$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$L$1 &amp; ", " &amp; $F$1 &amp; ") values (" &amp;A14 &amp; ", " &amp; B14 &amp; ", TO_DATE('" &amp; TEXT(F14, "DD/MM/YYYY") &amp; "', 'DD/MM/YYYY'));"</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO Delivery(OrderID, customer_nif, DateDelivery) values (7, 456, TO_DATE('26/09/YYYY', 'DD/MM/YYYY'));</v>
       </c>
       <c r="I14" t="str">
-        <f>"INSERT INTO " &amp; $I$1 &amp; "(" &amp; $K$1 &amp; ", " &amp;$M$1 &amp; ", " &amp; $D$1 &amp;") values (" &amp;A14 &amp; ", '" &amp; C14 &amp; "', " &amp; D14 &amp; ");"</f>
+        <f t="shared" si="2"/>
         <v>INSERT INTO ProductionOrder(OrderID, productcode, Quantity) values (7, 'AS12945S22', 8);</v>
       </c>
     </row>
@@ -3541,7 +3541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B436D-7E6F-45CD-A274-6E2AE1A9129E}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed errors in relational model and in excel
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\IdeaProjects\sem3pi2024_25_g125\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD4496-CE93-499E-AEB3-085C8EF13DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74785C6B-F970-4F98-B85C-D3DBE59A4DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="7" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="207">
   <si>
     <t>Name</t>
   </si>
@@ -625,18 +625,9 @@
     <t>WorkstationType_ID</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
     <t>Productcode</t>
   </si>
   <si>
-    <t>Partcode</t>
-  </si>
-  <si>
-    <t>Part</t>
-  </si>
-  <si>
     <t>ProductFamilyID</t>
   </si>
   <si>
@@ -659,6 +650,21 @@
   </si>
   <si>
     <t>OrderID</t>
+  </si>
+  <si>
+    <t>child_code</t>
+  </si>
+  <si>
+    <t>Product_BillOfMaterials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BillOfMaterialsparent_code </t>
+  </si>
+  <si>
+    <t>BillOfMaterialschild_code</t>
+  </si>
+  <si>
+    <t>parent_code</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1109,10 @@
         <v>186</v>
       </c>
       <c r="O1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="P1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -1268,7 +1274,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,7 +1298,7 @@
         <v>145</v>
       </c>
       <c r="E1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F1" t="s">
         <v>187</v>
@@ -1529,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE470C24-4865-4CED-BECB-9AD0BD718C1F}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,7 +1570,7 @@
         <v>129</v>
       </c>
       <c r="G1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H1" t="s">
         <v>177</v>
@@ -1576,7 +1582,7 @@
         <v>188</v>
       </c>
       <c r="K1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L1" t="s">
         <v>189</v>
@@ -2454,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
         <v>141</v>
@@ -3048,10 +3054,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D833FD3A-319E-497B-BBC6-9FC6F2F78F3D}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3059,11 +3065,15 @@
     <col min="1" max="1" width="14.21875" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" customWidth="1"/>
     <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="129.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="131.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -3077,22 +3087,28 @@
         <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="F1" t="s">
-        <v>181</v>
+        <v>203</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
       </c>
       <c r="H1" t="s">
         <v>193</v>
       </c>
       <c r="I1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="J1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="K1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3106,15 +3122,15 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <f>"INSERT INTO " &amp; $E$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$C$1 &amp; ") values ('" &amp; B2 &amp; "', '" &amp; C2 &amp; "');"</f>
-        <v>INSERT INTO Part(code, Description) values ('PN12344A21', 'Screw M6 35 mm');</v>
+        <f>"INSERT INTO " &amp; $E$1 &amp; "(" &amp;$G$1 &amp; ", " &amp;$I$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$D$1 &amp; ") values ('" &amp; A2 &amp; "', '" &amp; B2 &amp; "', '" &amp; C2 &amp; "', " &amp; D2 &amp; ");"</f>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN12344A21', 'Screw M6 35 mm', 1);</v>
       </c>
       <c r="F2" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$I$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$D$1 &amp; ") values ('" &amp; A2 &amp; "', '" &amp; B2 &amp; "', " &amp; D2 &amp; ");"</f>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S22', 'PN12344A21', 1);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A2 &amp; "', '" &amp; A2 &amp; "', '" &amp; B2 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN12344A21');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3128,15 +3144,15 @@
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E21" si="0">"INSERT INTO " &amp; $E$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$C$1 &amp; ") values ('" &amp; B3 &amp; "', '" &amp; C3 &amp; "');"</f>
-        <v>INSERT INTO Part(code, Description) values ('PN52384R50', '300x300 mm 5mm stainless steel sheet');</v>
+        <f t="shared" ref="E3:E21" si="0">"INSERT INTO " &amp; $E$1 &amp; "(" &amp;$G$1 &amp; ", " &amp;$I$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$D$1 &amp; ") values ('" &amp; A3 &amp; "', '" &amp; B3 &amp; "', '" &amp; C3 &amp; "', " &amp; D3 &amp; ");"</f>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN52384R50', '300x300 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F21" si="1">"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$I$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$D$1 &amp; ") values ('" &amp; A3 &amp; "', '" &amp; B3 &amp; "', " &amp; D3 &amp; ");"</f>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S22', 'PN52384R50', 1);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A3 &amp; "', '" &amp; A3 &amp; "', '" &amp; B3 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN52384R50');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3151,14 +3167,14 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN52384R10', '300x300 mm 1mm stainless steel sheet');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN52384R10', '300x300 mm 1mm stainless steel sheet', 1);</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S22', 'PN52384R10', 1);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A4 &amp; "', '" &amp; A4 &amp; "', '" &amp; B4 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN52384R10');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3173,14 +3189,14 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18544A21', 'Rivet 6 mm');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN18544A21', 'Rivet 6 mm', 4);</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S22', 'PN18544A21', 4);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A5 &amp; "', '" &amp; A5 &amp; "', '" &amp; B5 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN18544A21');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3195,14 +3211,14 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18544C21', 'Stainless steel handle model U6');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN18544C21', 'Stainless steel handle model U6', 2);</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S22', 'PN18544C21', 2);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A6 &amp; "', '" &amp; A6 &amp; "', '" &amp; B6 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN18544C21');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3217,14 +3233,14 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18324C54', 'Stainless steel handle model R12');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN18324C54', 'Stainless steel handle model R12', 1);</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S22', 'PN18324C54', 1);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A7 &amp; "', '" &amp; A7 &amp; "', '" &amp; B7 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN18324C54');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3239,14 +3255,14 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN12344A21', 'Screw M6 35 mm');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN12344A21', 'Screw M6 35 mm', 1);</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S20', 'PN12344A21', 1);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A8 &amp; "', '" &amp; A8 &amp; "', '" &amp; B8 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN12344A21');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3261,14 +3277,14 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN52384R50', '300x300 mm 5mm stainless steel sheet');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN52384R50', '300x300 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S20', 'PN52384R50', 1);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A9 &amp; "', '" &amp; A9 &amp; "', '" &amp; B9 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN52384R50');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3283,14 +3299,14 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN52384R10', '300x300 mm 1mm stainless steel sheet');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN52384R10', '300x300 mm 1mm stainless steel sheet', 1);</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S20', 'PN52384R10', 1);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A10 &amp; "', '" &amp; A10 &amp; "', '" &amp; B10 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN52384R10');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3305,14 +3321,14 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18544A21', 'Rivet 6 mm');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN18544A21', 'Rivet 6 mm', 4);</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S20', 'PN18544A21', 4);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A11 &amp; "', '" &amp; A11 &amp; "', '" &amp; B11 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN18544A21');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3327,14 +3343,14 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18544C21', 'Stainless steel handle model U6');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN18544C21', 'Stainless steel handle model U6', 2);</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S20', 'PN18544C21', 2);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A12 &amp; "', '" &amp; A12 &amp; "', '" &amp; B12 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN18544C21');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3349,14 +3365,14 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18324C51', 'Stainless steel handle model R11');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN18324C51', 'Stainless steel handle model R11', 1);</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S20', 'PN18324C51', 1);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A13 &amp; "', '" &amp; A13 &amp; "', '" &amp; B13 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN18324C51');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -3371,14 +3387,14 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN12344A21', 'Screw M6 35 mm');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN12344A21', 'Screw M6 35 mm', 1);</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S17', 'PN12344A21', 1);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A14 &amp; "', '" &amp; A14 &amp; "', '" &amp; B14 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN12344A21');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3393,14 +3409,14 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN52384R45', '250x250 mm 5mm stainless steel sheet');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN52384R45', '250x250 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S17', 'PN52384R45', 1);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A15 &amp; "', '" &amp; A15 &amp; "', '" &amp; B15 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN52384R45');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3415,11 +3431,11 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN52384R12', '250x250 mm 1mm stainless steel sheet');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN52384R12', '250x250 mm 1mm stainless steel sheet', 1);</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S17', 'PN52384R12', 1);</v>
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A16 &amp; "', '" &amp; A16 &amp; "', '" &amp; B16 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN52384R12');</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -3437,11 +3453,11 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18544A21', 'Rivet 6 mm');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN18544A21', 'Rivet 6 mm', 4);</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S17', 'PN18544A21', 4);</v>
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A17 &amp; "', '" &amp; A17 &amp; "', '" &amp; B17 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN18544A21');</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -3459,11 +3475,11 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18544C21', 'Stainless steel handle model U6');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN18544C21', 'Stainless steel handle model U6', 2);</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S17', 'PN18544C21', 2);</v>
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A18 &amp; "', '" &amp; A18 &amp; "', '" &amp; B18 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN18544C21');</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -3481,11 +3497,11 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18324C51', 'Stainless steel handle model R11');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN18324C51', 'Stainless steel handle model R11', 1);</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945S17', 'PN18324C51', 1);</v>
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A19 &amp; "', '" &amp; A19 &amp; "', '" &amp; B19 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN18324C51');</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -3503,11 +3519,11 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN52384R45', '250x250 mm 5mm stainless steel sheet');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945P17', 'PN52384R45', '250x250 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945P17', 'PN52384R45', 1);</v>
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A20 &amp; "', '" &amp; A20 &amp; "', '" &amp; B20 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945P17', 'AS12945P17', 'PN52384R45');</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3525,11 +3541,11 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Part(code, Description) values ('PN18324C91', 'Stainless steel handle model S26');</v>
+        <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945P17', 'PN18324C91', 'Stainless steel handle model S26', 1);</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO BillOfMaterials(Productcode, Partcode, Quantity) values ('AS12945P17', 'PN18324C91', 1);</v>
+        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A21 &amp; "', '" &amp; A21 &amp; "', '" &amp; B21 &amp; "');"</f>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945P17', 'AS12945P17', 'PN18324C91');</v>
       </c>
     </row>
   </sheetData>
@@ -3542,7 +3558,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3568,13 +3584,13 @@
         <v>180</v>
       </c>
       <c r="F1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Final changes to excel
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\IdeaProjects\sem3pi2024_25_g125\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74785C6B-F970-4F98-B85C-D3DBE59A4DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A5051B-3858-4160-8E37-D404FB21FE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="7" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="4" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -1273,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15D9EF7-7F05-4929-9267-83A028A1D45D}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1535,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE470C24-4865-4CED-BECB-9AD0BD718C1F}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2016,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8F968F-3FE6-476E-97DD-6EBBFE3BD57E}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2442,7 +2442,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3056,8 +3056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D833FD3A-319E-497B-BBC6-9FC6F2F78F3D}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3558,7 +3558,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added folder for sprint 2
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\IdeaProjects\sem3pi2024_25_g125\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A5051B-3858-4160-8E37-D404FB21FE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19CB475-469A-4168-B16E-D5C3412208CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="4" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="7" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D52B8C6-F495-435D-B053-FB604FC6DD2C}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K5"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2016,7 +2016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8F968F-3FE6-476E-97DD-6EBBFE3BD57E}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3054,10 +3054,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D833FD3A-319E-497B-BBC6-9FC6F2F78F3D}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3126,7 +3126,7 @@
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN12344A21', 'Screw M6 35 mm', 1);</v>
       </c>
       <c r="F2" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A2 &amp; "', '" &amp; A2 &amp; "', '" &amp; B2 &amp; "');"</f>
+        <f t="shared" ref="F2:F22" si="0">"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A2 &amp; "', '" &amp; A2 &amp; "', '" &amp; B2 &amp; "');"</f>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN12344A21');</v>
       </c>
     </row>
@@ -3144,11 +3144,11 @@
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E21" si="0">"INSERT INTO " &amp; $E$1 &amp; "(" &amp;$G$1 &amp; ", " &amp;$I$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$D$1 &amp; ") values ('" &amp; A3 &amp; "', '" &amp; B3 &amp; "', '" &amp; C3 &amp; "', " &amp; D3 &amp; ");"</f>
+        <f t="shared" ref="E3:E21" si="1">"INSERT INTO " &amp; $E$1 &amp; "(" &amp;$G$1 &amp; ", " &amp;$I$1 &amp; ", " &amp;$C$1 &amp; ", " &amp;$D$1 &amp; ") values ('" &amp; A3 &amp; "', '" &amp; B3 &amp; "', '" &amp; C3 &amp; "', " &amp; D3 &amp; ");"</f>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN52384R50', '300x300 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F3" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A3 &amp; "', '" &amp; A3 &amp; "', '" &amp; B3 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN52384R50');</v>
       </c>
     </row>
@@ -3166,11 +3166,11 @@
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN52384R10', '300x300 mm 1mm stainless steel sheet', 1);</v>
       </c>
       <c r="F4" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A4 &amp; "', '" &amp; A4 &amp; "', '" &amp; B4 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN52384R10');</v>
       </c>
     </row>
@@ -3188,11 +3188,11 @@
         <v>4</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN18544A21', 'Rivet 6 mm', 4);</v>
       </c>
       <c r="F5" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A5 &amp; "', '" &amp; A5 &amp; "', '" &amp; B5 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN18544A21');</v>
       </c>
     </row>
@@ -3210,11 +3210,11 @@
         <v>2</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN18544C21', 'Stainless steel handle model U6', 2);</v>
       </c>
       <c r="F6" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A6 &amp; "', '" &amp; A6 &amp; "', '" &amp; B6 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN18544C21');</v>
       </c>
     </row>
@@ -3232,11 +3232,11 @@
         <v>1</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S22', 'PN18324C54', 'Stainless steel handle model R12', 1);</v>
       </c>
       <c r="F7" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A7 &amp; "', '" &amp; A7 &amp; "', '" &amp; B7 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S22', 'AS12945S22', 'PN18324C54');</v>
       </c>
     </row>
@@ -3254,11 +3254,11 @@
         <v>1</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN12344A21', 'Screw M6 35 mm', 1);</v>
       </c>
       <c r="F8" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A8 &amp; "', '" &amp; A8 &amp; "', '" &amp; B8 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN12344A21');</v>
       </c>
     </row>
@@ -3276,11 +3276,11 @@
         <v>1</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN52384R50', '300x300 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F9" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A9 &amp; "', '" &amp; A9 &amp; "', '" &amp; B9 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN52384R50');</v>
       </c>
     </row>
@@ -3298,11 +3298,11 @@
         <v>1</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN52384R10', '300x300 mm 1mm stainless steel sheet', 1);</v>
       </c>
       <c r="F10" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A10 &amp; "', '" &amp; A10 &amp; "', '" &amp; B10 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN52384R10');</v>
       </c>
     </row>
@@ -3320,11 +3320,11 @@
         <v>4</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN18544A21', 'Rivet 6 mm', 4);</v>
       </c>
       <c r="F11" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A11 &amp; "', '" &amp; A11 &amp; "', '" &amp; B11 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN18544A21');</v>
       </c>
     </row>
@@ -3342,11 +3342,11 @@
         <v>2</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN18544C21', 'Stainless steel handle model U6', 2);</v>
       </c>
       <c r="F12" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A12 &amp; "', '" &amp; A12 &amp; "', '" &amp; B12 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN18544C21');</v>
       </c>
     </row>
@@ -3364,11 +3364,11 @@
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S20', 'PN18324C51', 'Stainless steel handle model R11', 1);</v>
       </c>
       <c r="F13" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A13 &amp; "', '" &amp; A13 &amp; "', '" &amp; B13 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S20', 'AS12945S20', 'PN18324C51');</v>
       </c>
     </row>
@@ -3386,11 +3386,11 @@
         <v>1</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN12344A21', 'Screw M6 35 mm', 1);</v>
       </c>
       <c r="F14" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A14 &amp; "', '" &amp; A14 &amp; "', '" &amp; B14 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN12344A21');</v>
       </c>
     </row>
@@ -3408,11 +3408,11 @@
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN52384R45', '250x250 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F15" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A15 &amp; "', '" &amp; A15 &amp; "', '" &amp; B15 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN52384R45');</v>
       </c>
     </row>
@@ -3430,11 +3430,11 @@
         <v>1</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN52384R12', '250x250 mm 1mm stainless steel sheet', 1);</v>
       </c>
       <c r="F16" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A16 &amp; "', '" &amp; A16 &amp; "', '" &amp; B16 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN52384R12');</v>
       </c>
     </row>
@@ -3452,11 +3452,11 @@
         <v>4</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN18544A21', 'Rivet 6 mm', 4);</v>
       </c>
       <c r="F17" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A17 &amp; "', '" &amp; A17 &amp; "', '" &amp; B17 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN18544A21');</v>
       </c>
     </row>
@@ -3474,11 +3474,11 @@
         <v>2</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN18544C21', 'Stainless steel handle model U6', 2);</v>
       </c>
       <c r="F18" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A18 &amp; "', '" &amp; A18 &amp; "', '" &amp; B18 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN18544C21');</v>
       </c>
     </row>
@@ -3496,11 +3496,11 @@
         <v>1</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945S17', 'PN18324C51', 'Stainless steel handle model R11', 1);</v>
       </c>
       <c r="F19" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A19 &amp; "', '" &amp; A19 &amp; "', '" &amp; B19 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945S17', 'AS12945S17', 'PN18324C51');</v>
       </c>
     </row>
@@ -3518,11 +3518,11 @@
         <v>1</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945P17', 'PN52384R45', '250x250 mm 5mm stainless steel sheet', 1);</v>
       </c>
       <c r="F20" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A20 &amp; "', '" &amp; A20 &amp; "', '" &amp; B20 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945P17', 'AS12945P17', 'PN52384R45');</v>
       </c>
     </row>
@@ -3540,12 +3540,18 @@
         <v>1</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO BillOfMaterials(parent_code, child_code, Description, Quantity) values ('AS12945P17', 'PN18324C91', 'Stainless steel handle model S26', 1);</v>
       </c>
       <c r="F21" t="str">
-        <f>"INSERT INTO " &amp; $F$1 &amp; "(" &amp;$H$1 &amp; ", " &amp;$J$1 &amp; ", " &amp;$K$1 &amp; ") values ('" &amp; A21 &amp; "', '" &amp; A21 &amp; "', '" &amp; B21 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('AS12945P17', 'AS12945P17', 'PN18324C91');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Product_BillOfMaterials(Productcode, BillOfMaterialsparent_code , BillOfMaterialschild_code) values ('', '', '');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>